<commit_message>
Se agrego la grafica y como se inicia el proyecto
</commit_message>
<xml_diff>
--- a/final_data/Final_date.xlsx
+++ b/final_data/Final_date.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,456 +458,416 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Andres</t>
+          <t>Daniela</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gil</t>
+          <t>Villamizar</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3193228813</v>
+        <v>3218490916</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12/01/2023</t>
+          <t>12/02/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sebasti4n</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cortes</t>
+          <t>Botero</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3226803059</v>
+        <v>3218748814</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>25/06/2023</t>
+          <t>13/02/2022</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Manuela</t>
+          <t>Cristian</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Correa</t>
+          <t>Solarte</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3185957386</v>
+        <v>3148227994</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>14/02/2022</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jacobo</t>
+          <t>Julian</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Montenegro</t>
+          <t>Aristizabal</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3233073789</v>
+        <v>3046145922</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>08/04/2022</t>
+          <t>15/02/2022</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Carvajal</t>
+          <t>Londoño</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3235837848</v>
+        <v>3163610054</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>16/02/2022</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Mauricio</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Carvajal</t>
+          <t>Herrera</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3193917279</v>
+        <v>3117754781</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>19/12/2024</t>
+          <t>17/02/2022</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samuel</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>Esteban</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Meneses</t>
+        </is>
+      </c>
       <c r="C8" t="n">
-        <v>28304</v>
+        <v>3108017554</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>02/04/2023</t>
+          <t>18/02/2022</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Juan Jose</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Paraco</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3165326067</v>
+        <v>3188288098</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>17/11/2023</t>
+          <t>19/02/2022</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Lina</t>
+          <t>Alejandra</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Franco</t>
+          <t>Ruiz</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3157266898</v>
+        <v>3167357054</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>02/10/2023</t>
+          <t>20/02/2022</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hugo </t>
+          <t>Daniela</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>Bustos</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3015698423</v>
+        <v>3164224295</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12/02/2022</t>
+          <t>21/02/2022</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Martín </t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Martinez</t>
+          <t>Hoyos</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3215698521</v>
+        <v>3113829197</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>16/03/2022</t>
+          <t>22/02/2022</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lucas </t>
+          <t>Manuela</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Rojas</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3136482105</v>
+        <v>3114244572</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>23/02/2022</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mateo </t>
+          <t>Andres</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Gil</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3145678015</v>
+        <v>3193228813</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>15/09/2024</t>
+          <t>12/01/2023</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leo </t>
+          <t>Sebasti4n</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lopez</t>
+          <t>Cortes</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3116254231</v>
+        <v>3226803059</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>09/08/2023</t>
+          <t>25/06/2023</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel </t>
+          <t>Manuela</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Gonzalez</t>
+          <t>Correa</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3002016952</v>
+        <v>3185957386</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22/06/2023</t>
+          <t>12/10/2024</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alejandro </t>
+          <t>Jacobo</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3023519754</v>
+        <v>3233073789</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>18/11/2024</t>
+          <t>08/04/2022</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pablo </t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sanchez</t>
+          <t>Carvajal</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3015698567</v>
+        <v>3235837848</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>23/04/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Manuel</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Perez</t>
+          <t>Carvajal</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3236521693</v>
+        <v>3193917279</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>09/04/2022</t>
+          <t>19/12/2024</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Álvaro </t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Valencia</t>
-        </is>
-      </c>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="n">
-        <v>3189657436</v>
+        <v>28304</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14/06/2023</t>
+          <t>02/04/2023</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adrián </t>
+          <t>Juan Jose</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Duque</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3185201260</v>
+        <v>3165326067</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>25/07/2024</t>
+          <t>17/11/2023</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">David </t>
+          <t>Lina</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Perdomo</t>
+          <t>Franco</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3224697851</v>
+        <v>3157266898</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>24/02/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mario </t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Cardona</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>3230569853</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>28/10/2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enzo </t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Arango</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>3045876320</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>12/09/2023</t>
+          <t>02/10/2023</t>
         </is>
       </c>
     </row>

</xml_diff>